<commit_message>
Poorva files uploaded on 10/04/2018
</commit_message>
<xml_diff>
--- a/test data/data.xlsx
+++ b/test data/data.xlsx
@@ -13,12 +13,11 @@
     <sheet name="eventdetails" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="C1:P7"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
   <si>
     <t>Consignment Number</t>
   </si>
@@ -30,6 +29,18 @@
   </si>
   <si>
     <t>PREC01048239</t>
+  </si>
+  <si>
+    <t>Reshma</t>
+  </si>
+  <si>
+    <t>Ayesha</t>
+  </si>
+  <si>
+    <t>CARDITRECEPTACLEID00000111037</t>
+  </si>
+  <si>
+    <t>Heena</t>
   </si>
 </sst>
 </file>
@@ -368,40 +379,59 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A11"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" customWidth="1"/>
+    <col min="7" max="7" width="30.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>4</v>
+      </c>
+      <c r="F12" t="s">
+        <v>3</v>
+      </c>
+      <c r="G12" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
poorva files uploaded on 10/08/2018
</commit_message>
<xml_diff>
--- a/test data/data.xlsx
+++ b/test data/data.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>PREC01048239</t>
   </si>
@@ -35,6 +35,18 @@
   </si>
   <si>
     <t>CARDITRECEPTACLEID00000111201</t>
+  </si>
+  <si>
+    <t>AllOntime</t>
+  </si>
+  <si>
+    <t>PREC01049379</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>PRECON</t>
   </si>
 </sst>
 </file>
@@ -373,10 +385,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -388,7 +400,7 @@
     <col min="7" max="7" width="30.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -398,8 +410,11 @@
       <c r="C1" t="s">
         <v>3</v>
       </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -408,6 +423,17 @@
       </c>
       <c r="C2" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Poorva updated on 10/10/2018
</commit_message>
<xml_diff>
--- a/test data/data.xlsx
+++ b/test data/data.xlsx
@@ -4,23 +4,24 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="13620" windowHeight="2580"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="13620" windowHeight="2580" firstSheet="3" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="1" r:id="rId1"/>
     <sheet name="consignmentsummary" sheetId="2" r:id="rId2"/>
-    <sheet name="precondetails" sheetId="3" r:id="rId3"/>
-    <sheet name="eventdetails" sheetId="4" r:id="rId4"/>
+    <sheet name="mailclassinfotable" sheetId="7" r:id="rId3"/>
+    <sheet name="handoverinfotable" sheetId="8" r:id="rId4"/>
+    <sheet name="cardittransporttable" sheetId="9" r:id="rId5"/>
+    <sheet name="eventinfotable" sheetId="10" r:id="rId6"/>
+    <sheet name="precontransporttable" sheetId="11" r:id="rId7"/>
+    <sheet name="receptacleinfotable" sheetId="12" r:id="rId8"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
-  <si>
-    <t>PREC01048239</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="109">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -34,19 +35,319 @@
     <t>CommonTestData</t>
   </si>
   <si>
-    <t>CARDITRECEPTACLEID00000111201</t>
-  </si>
-  <si>
     <t>AllOntime</t>
   </si>
   <si>
-    <t>PREC01049379</t>
-  </si>
-  <si>
-    <t>Status</t>
-  </si>
-  <si>
     <t>PRECON</t>
+  </si>
+  <si>
+    <t>Event_NA</t>
+  </si>
+  <si>
+    <t>Event_Delivered</t>
+  </si>
+  <si>
+    <t>Event_Received</t>
+  </si>
+  <si>
+    <t>Event_Enroute</t>
+  </si>
+  <si>
+    <t>Event_Cardit</t>
+  </si>
+  <si>
+    <t>Event_Precon</t>
+  </si>
+  <si>
+    <t>FULL</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>RECEIVED ON TIME</t>
+  </si>
+  <si>
+    <t>DELIVERED ON TIME</t>
+  </si>
+  <si>
+    <t>Delivered (21)</t>
+  </si>
+  <si>
+    <t>HANDOVER ON TIME</t>
+  </si>
+  <si>
+    <t>Received (74)</t>
+  </si>
+  <si>
+    <t>ENROUTE</t>
+  </si>
+  <si>
+    <t>En route (31)</t>
+  </si>
+  <si>
+    <t>CREATED</t>
+  </si>
+  <si>
+    <t>CARDIT(9)</t>
+  </si>
+  <si>
+    <t>PRECON(14)</t>
+  </si>
+  <si>
+    <t>Consignment_Status_Precon</t>
+  </si>
+  <si>
+    <t>Consignment_Status_Cardit</t>
+  </si>
+  <si>
+    <t>Consignment_Status_Enroute</t>
+  </si>
+  <si>
+    <t>Consignment_Status_Received</t>
+  </si>
+  <si>
+    <t>Consignment_Status_Delivered</t>
+  </si>
+  <si>
+    <t>Consignment_Status_NA</t>
+  </si>
+  <si>
+    <t>Count_Flag_N</t>
+  </si>
+  <si>
+    <t>Count_Flag_F</t>
+  </si>
+  <si>
+    <t>AllLateDiscrepancy</t>
+  </si>
+  <si>
+    <t>HANDOVER LATE</t>
+  </si>
+  <si>
+    <t>Count_Flag_D</t>
+  </si>
+  <si>
+    <t>DISCREPANCY</t>
+  </si>
+  <si>
+    <t>DELIVERED LATE</t>
+  </si>
+  <si>
+    <t>RECEIVED LATE</t>
+  </si>
+  <si>
+    <t>PREC01050308</t>
+  </si>
+  <si>
+    <t>RESCON RECEIVED</t>
+  </si>
+  <si>
+    <t>PREC01050310</t>
+  </si>
+  <si>
+    <t>AllUnknown</t>
+  </si>
+  <si>
+    <t>PREC01050311</t>
+  </si>
+  <si>
+    <t>HANDOVER UNKNOWN</t>
+  </si>
+  <si>
+    <t>DELIVERED UNKNOWN</t>
+  </si>
+  <si>
+    <t>RECEIVED UNKNOWN</t>
+  </si>
+  <si>
+    <t>CARDITRECEPTACLEID00000111316</t>
+  </si>
+  <si>
+    <t>AllDelayed</t>
+  </si>
+  <si>
+    <t>HANDOVER DELAYED (sys)</t>
+  </si>
+  <si>
+    <t>HANDOVER DELAYED</t>
+  </si>
+  <si>
+    <t>DELIVERY DELAYED(sys)</t>
+  </si>
+  <si>
+    <t>DELIVERY DELAYED</t>
+  </si>
+  <si>
+    <t>RECEIVED DELAYED (sys)</t>
+  </si>
+  <si>
+    <t>RECEIVED DELAYED</t>
+  </si>
+  <si>
+    <t>Cstatus</t>
+  </si>
+  <si>
+    <t>CCompDate</t>
+  </si>
+  <si>
+    <t>Ccategory</t>
+  </si>
+  <si>
+    <t>Cdest</t>
+  </si>
+  <si>
+    <t>MailClassL</t>
+  </si>
+  <si>
+    <t>MailClassE</t>
+  </si>
+  <si>
+    <t>MailClassU</t>
+  </si>
+  <si>
+    <t>TotalCountL</t>
+  </si>
+  <si>
+    <t>TotalCountE</t>
+  </si>
+  <si>
+    <t>TotalCountU</t>
+  </si>
+  <si>
+    <t>WeightL</t>
+  </si>
+  <si>
+    <t>WeightE</t>
+  </si>
+  <si>
+    <t>WeightU</t>
+  </si>
+  <si>
+    <t>HOLC</t>
+  </si>
+  <si>
+    <t>HOCO</t>
+  </si>
+  <si>
+    <t>HDLC</t>
+  </si>
+  <si>
+    <t>HDCO</t>
+  </si>
+  <si>
+    <t>TQ</t>
+  </si>
+  <si>
+    <t>TCR</t>
+  </si>
+  <si>
+    <t>TDLC</t>
+  </si>
+  <si>
+    <t>TALC</t>
+  </si>
+  <si>
+    <t>TDDT</t>
+  </si>
+  <si>
+    <t>TADT</t>
+  </si>
+  <si>
+    <t>Event</t>
+  </si>
+  <si>
+    <t>EDT</t>
+  </si>
+  <si>
+    <t>ECS</t>
+  </si>
+  <si>
+    <t>ECF</t>
+  </si>
+  <si>
+    <t>EL</t>
+  </si>
+  <si>
+    <t>TM</t>
+  </si>
+  <si>
+    <t>TCC</t>
+  </si>
+  <si>
+    <t>RecpID</t>
+  </si>
+  <si>
+    <t>RCJID</t>
+  </si>
+  <si>
+    <t>RCID</t>
+  </si>
+  <si>
+    <t>RCS</t>
+  </si>
+  <si>
+    <t>Letters (LC/AO)</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>EMS</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>LHR</t>
+  </si>
+  <si>
+    <t>10-10-18 08:10</t>
+  </si>
+  <si>
+    <t>PHC</t>
+  </si>
+  <si>
+    <t>10-10-18 12:36</t>
+  </si>
+  <si>
+    <t>Main-Carriage (20)</t>
+  </si>
+  <si>
+    <t>AC865</t>
+  </si>
+  <si>
+    <t>10-10-18 07:06</t>
+  </si>
+  <si>
+    <t>10-10-18 07:09</t>
+  </si>
+  <si>
+    <t>CARDITRECEPTACLEID00000111334</t>
+  </si>
+  <si>
+    <t>CONTAINERJOURID312</t>
+  </si>
+  <si>
+    <t>RecpWt</t>
+  </si>
+  <si>
+    <t>CONTAINERNO91</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>NGPHCA</t>
+  </si>
+  <si>
+    <t>CARDITFieldValidations</t>
   </si>
 </sst>
 </file>
@@ -82,8 +383,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -385,55 +688,255 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:R6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.28515625" customWidth="1"/>
     <col min="3" max="3" width="30.5703125" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" customWidth="1"/>
+    <col min="5" max="5" width="26.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.140625" customWidth="1"/>
-    <col min="7" max="7" width="30.85546875" customWidth="1"/>
+    <col min="7" max="7" width="26" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.140625" customWidth="1"/>
+    <col min="18" max="18" width="16.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>27</v>
+      </c>
+      <c r="L1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M1" t="s">
+        <v>28</v>
+      </c>
+      <c r="N1" t="s">
+        <v>6</v>
+      </c>
+      <c r="O1" t="s">
+        <v>29</v>
+      </c>
+      <c r="P1" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>31</v>
+      </c>
+      <c r="R1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="B3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" t="s">
-        <v>9</v>
+      <c r="F3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K3" t="s">
+        <v>17</v>
+      </c>
+      <c r="L3" t="s">
+        <v>16</v>
+      </c>
+      <c r="M3" t="s">
+        <v>15</v>
+      </c>
+      <c r="N3" t="s">
+        <v>39</v>
+      </c>
+      <c r="O3" t="s">
+        <v>14</v>
+      </c>
+      <c r="P3" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" t="s">
+        <v>40</v>
+      </c>
+      <c r="F4" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I4" t="s">
+        <v>19</v>
+      </c>
+      <c r="J4" t="s">
+        <v>18</v>
+      </c>
+      <c r="K4" t="s">
+        <v>33</v>
+      </c>
+      <c r="L4" t="s">
+        <v>16</v>
+      </c>
+      <c r="M4" t="s">
+        <v>36</v>
+      </c>
+      <c r="N4" t="s">
+        <v>39</v>
+      </c>
+      <c r="O4" t="s">
+        <v>37</v>
+      </c>
+      <c r="P4" t="s">
+        <v>13</v>
+      </c>
+      <c r="R4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" t="s">
+        <v>42</v>
+      </c>
+      <c r="J5" t="s">
+        <v>18</v>
+      </c>
+      <c r="K5" t="s">
+        <v>43</v>
+      </c>
+      <c r="L5" t="s">
+        <v>16</v>
+      </c>
+      <c r="M5" t="s">
+        <v>44</v>
+      </c>
+      <c r="N5" t="s">
+        <v>39</v>
+      </c>
+      <c r="O5" t="s">
+        <v>45</v>
+      </c>
+      <c r="P5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6" t="s">
+        <v>42</v>
+      </c>
+      <c r="F6" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" t="s">
+        <v>21</v>
+      </c>
+      <c r="J6" t="s">
+        <v>48</v>
+      </c>
+      <c r="K6" t="s">
+        <v>49</v>
+      </c>
+      <c r="L6" t="s">
+        <v>50</v>
+      </c>
+      <c r="M6" t="s">
+        <v>51</v>
+      </c>
+      <c r="N6" t="s">
+        <v>52</v>
+      </c>
+      <c r="O6" t="s">
+        <v>53</v>
+      </c>
+      <c r="P6" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -443,38 +946,447 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" s="2">
+        <v>43383.295138888891</v>
+      </c>
+      <c r="E2" t="s">
+        <v>106</v>
+      </c>
+      <c r="F2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="18.85546875" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G1" t="s">
+        <v>63</v>
+      </c>
+      <c r="H1" t="s">
+        <v>64</v>
+      </c>
+      <c r="I1" t="s">
+        <v>65</v>
+      </c>
+      <c r="J1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D2" t="s">
+        <v>96</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="13.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F1" t="s">
+        <v>75</v>
+      </c>
+      <c r="G1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E2" t="s">
+        <v>96</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.42578125" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F1" t="s">
+        <v>80</v>
+      </c>
+      <c r="G1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="2">
+        <v>43383.295138888891</v>
+      </c>
+      <c r="E2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1" t="s">
+        <v>104</v>
+      </c>
+      <c r="E1" t="s">
+        <v>86</v>
+      </c>
+      <c r="F1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D2">
+        <v>6.2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>